<commit_message>
Added 3d scanner slides for market analysis
</commit_message>
<xml_diff>
--- a/docs/products/3dtools.xlsx
+++ b/docs/products/3dtools.xlsx
@@ -10,14 +10,14 @@
     <sheet name="3D Tools" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3D Tools'!$A$1:$I$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3D Tools'!$A$2:$I$117</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196">
   <si>
     <t>Product Name</t>
   </si>
@@ -52,16 +52,25 @@
     <t>Parametric</t>
   </si>
   <si>
+    <t>3D Sprint</t>
+  </si>
+  <si>
+    <t>3D System</t>
+  </si>
+  <si>
+    <t>3D Printing</t>
+  </si>
+  <si>
+    <t>√</t>
+  </si>
+  <si>
     <t>3D View/Build</t>
   </si>
   <si>
     <t>Microsoft</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>√</t>
+    <t>Model Viewer</t>
   </si>
   <si>
     <t>3D-matic</t>
@@ -97,6 +106,9 @@
     <t>Scene Composer</t>
   </si>
   <si>
+    <t>3DXpert</t>
+  </si>
+  <si>
     <t>Alias Design</t>
   </si>
   <si>
@@ -151,6 +163,9 @@
     <t>NewTek</t>
   </si>
   <si>
+    <t>CimatronE</t>
+  </si>
+  <si>
     <t>Cinema 4D Studio</t>
   </si>
   <si>
@@ -166,54 +181,48 @@
     <t>Exocortex Technologies</t>
   </si>
   <si>
-    <t>ClayTools</t>
+    <t>Cobalt</t>
+  </si>
+  <si>
+    <t>Ashlar-Vellum</t>
+  </si>
+  <si>
+    <t>CraftWare</t>
+  </si>
+  <si>
+    <t>Craft Unique</t>
+  </si>
+  <si>
+    <t>CryEngine</t>
+  </si>
+  <si>
+    <t>Crytek</t>
+  </si>
+  <si>
+    <t>Cura</t>
+  </si>
+  <si>
+    <t>Ultimaker</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D3JS</t>
+  </si>
+  <si>
+    <t>SVG Library</t>
+  </si>
+  <si>
+    <t>DAZ Studio Pro</t>
+  </si>
+  <si>
+    <t>DesignX</t>
   </si>
   <si>
     <t xml:space="preserve">Geomagic  </t>
   </si>
   <si>
-    <t>Cobalt</t>
-  </si>
-  <si>
-    <t>Ashlar-Vellum</t>
-  </si>
-  <si>
-    <t>CraftWare</t>
-  </si>
-  <si>
-    <t>Craft Unique</t>
-  </si>
-  <si>
-    <t>3D Printing</t>
-  </si>
-  <si>
-    <t>CryEngine</t>
-  </si>
-  <si>
-    <t>Crytek</t>
-  </si>
-  <si>
-    <t>Cura</t>
-  </si>
-  <si>
-    <t>Ultimaker</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D3JS</t>
-  </si>
-  <si>
-    <t>SVG Library</t>
-  </si>
-  <si>
-    <t>DAZ Studio Pro</t>
-  </si>
-  <si>
-    <t>DesignX</t>
-  </si>
-  <si>
     <t>DraftSight</t>
   </si>
   <si>
@@ -247,7 +256,7 @@
     <t>FreeCAD</t>
   </si>
   <si>
-    <t>Freeform Plus</t>
+    <t>Freeform</t>
   </si>
   <si>
     <t>Fusion 360</t>
@@ -259,9 +268,6 @@
     <t>Stratasys</t>
   </si>
   <si>
-    <t>Model Viewer</t>
-  </si>
-  <si>
     <t>Grasshopper</t>
   </si>
   <si>
@@ -301,6 +307,12 @@
     <t>Image Library</t>
   </si>
   <si>
+    <t>itSeez3D</t>
+  </si>
+  <si>
+    <t>Photogrammetry</t>
+  </si>
+  <si>
     <t>JointJS</t>
   </si>
   <si>
@@ -397,6 +409,12 @@
     <t>Sencha</t>
   </si>
   <si>
+    <t>Photoscan</t>
+  </si>
+  <si>
+    <t>Agisoft</t>
+  </si>
+  <si>
     <t>PIXLR</t>
   </si>
   <si>
@@ -424,12 +442,15 @@
     <t>PTC</t>
   </si>
   <si>
+    <t>RealityCapture</t>
+  </si>
+  <si>
+    <t>CapturingReality</t>
+  </si>
+  <si>
     <t>Recap</t>
   </si>
   <si>
-    <t>Photogrammetry</t>
-  </si>
-  <si>
     <t>Remake</t>
   </si>
   <si>
@@ -445,6 +466,18 @@
     <t>Scaleform</t>
   </si>
   <si>
+    <t>Scandy</t>
+  </si>
+  <si>
+    <t>Scann3D</t>
+  </si>
+  <si>
+    <t>SmartMobileVision</t>
+  </si>
+  <si>
+    <t>Sculpt</t>
+  </si>
+  <si>
     <t>Sculptris</t>
   </si>
   <si>
@@ -493,6 +526,12 @@
     <t>Solidworks Visualization</t>
   </si>
   <si>
+    <t>Source SDK</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
     <t>Three.js</t>
   </si>
   <si>
@@ -505,6 +544,9 @@
     <t>Tinkercad</t>
   </si>
   <si>
+    <t>Trimensional</t>
+  </si>
+  <si>
     <t>Turbulenz</t>
   </si>
   <si>
@@ -538,13 +580,31 @@
     <t xml:space="preserve">VXmodel </t>
   </si>
   <si>
-    <t>CREATFORM</t>
+    <t>Createform</t>
   </si>
   <si>
     <t>Within</t>
   </si>
   <si>
+    <t>Wrap</t>
+  </si>
+  <si>
+    <t>XYZMaker</t>
+  </si>
+  <si>
+    <t>XYZPrinting</t>
+  </si>
+  <si>
+    <t>XYZPhoto</t>
+  </si>
+  <si>
     <t>Zbrush</t>
+  </si>
+  <si>
+    <t>Zephyr</t>
+  </si>
+  <si>
+    <t>3DFlow</t>
   </si>
 </sst>
 </file>
@@ -585,9 +645,24 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -601,39 +676,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -648,7 +692,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -663,43 +707,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -716,6 +723,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -723,7 +751,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -756,7 +816,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -768,7 +834,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -780,37 +954,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -822,115 +984,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -968,30 +1028,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1007,6 +1043,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1018,6 +1072,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1040,28 +1105,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1070,7 +1130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1088,130 +1148,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1560,14 +1620,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B102" activePane="bottomRight" state="frozenSplit"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D109" sqref="D109"/>
+      <selection pane="bottomRight" activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1657,12 +1717,12 @@
         <v>17</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9">
@@ -1673,7 +1733,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1681,29 +1741,27 @@
       <c r="G5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
@@ -1716,97 +1774,103 @@
         <v>25</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
+      <c r="A10" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="I10" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="I11" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1816,35 +1880,31 @@
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="5"/>
+      <c r="C13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="7"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="4" t="s">
-        <v>36</v>
+      <c r="A14" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1858,10 +1918,10 @@
         <v>39</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="7" t="s">
@@ -1872,45 +1932,41 @@
       <c r="H15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="8"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="7" t="s">
         <v>14</v>
       </c>
@@ -1918,60 +1974,64 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="5"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="E19" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F19" s="5"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="7" t="s">
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1980,17 +2040,17 @@
         <v>49</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="G21" s="8"/>
       <c r="H21" s="7" t="s">
         <v>14</v>
       </c>
@@ -1998,129 +2058,133 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="C23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="I23" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="I24" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="G25" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="4" t="s">
-        <v>63</v>
+      <c r="A27" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="8"/>
+        <v>61</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="8"/>
     </row>
     <row r="29" spans="1:9">
@@ -2128,10 +2192,10 @@
         <v>65</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -2142,21 +2206,23 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="8"/>
+      <c r="H30" s="7"/>
       <c r="I30" s="7" t="s">
         <v>14</v>
       </c>
@@ -2166,48 +2232,52 @@
         <v>68</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>70</v>
+      <c r="B32" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="8"/>
+      <c r="G32" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
+      <c r="I32" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>14</v>
@@ -2221,35 +2291,31 @@
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>74</v>
+      <c r="B34" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
       <c r="I34" s="8"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="9" t="s">
-        <v>75</v>
+      <c r="A35" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>14</v>
@@ -2267,10 +2333,10 @@
         <v>76</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -2284,79 +2350,83 @@
       <c r="I36" s="8"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="4" t="s">
-        <v>77</v>
+      <c r="A37" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
       <c r="I37" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="E38" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F38" s="5"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="9" t="s">
+      <c r="B40" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="C40" s="5" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -2370,27 +2440,31 @@
         <v>83</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
+      <c r="I41" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>21</v>
+      <c r="B42" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -2404,10 +2478,10 @@
         <v>85</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -2418,132 +2492,132 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
-      <c r="I45" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="I45" s="8"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="8"/>
+      <c r="G46" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H46" s="8"/>
-      <c r="I46" s="7" t="s">
+      <c r="I46" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
+      <c r="B47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
+      <c r="I47" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>95</v>
+      <c r="A48" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
+      <c r="I48" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="4" t="s">
-        <v>96</v>
+      <c r="A49" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="D50" s="5"/>
-      <c r="E50" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="E50" s="6"/>
       <c r="F50" s="5"/>
-      <c r="G50" s="8"/>
+      <c r="G50" s="6"/>
       <c r="H50" s="7" t="s">
         <v>14</v>
       </c>
@@ -2551,30 +2625,30 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
+      <c r="C51" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="C52" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -2585,61 +2659,57 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E53" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F53" s="5"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="H53" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H54" s="6"/>
+      <c r="C54" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
       <c r="I54" s="8"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C55" s="5" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H55" s="6"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
       <c r="I55" s="8"/>
     </row>
     <row r="56" spans="1:9">
@@ -2647,52 +2717,50 @@
         <v>107</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D57" s="5"/>
-      <c r="E57" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="E57" s="5"/>
       <c r="F57" s="5"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G57" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="6"/>
       <c r="I57" s="8"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -2705,110 +2773,116 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
+      <c r="E59" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F59" s="5"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
+      <c r="H59" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="I59" s="8"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E60" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F60" s="5"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G60" s="6"/>
+      <c r="H60" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="8"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" s="6"/>
+      <c r="I61" s="8"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C61" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>115</v>
+      <c r="B62" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
-      <c r="I62" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="I62" s="8"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
+      <c r="C63" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
+      <c r="I63" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
+      <c r="C64" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
@@ -2818,107 +2892,109 @@
         <v>119</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="6" t="s">
-        <v>14</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="8"/>
       <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
+      <c r="I65" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="6" t="s">
-        <v>14</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
+      <c r="A67" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="8"/>
+      <c r="A68" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
+        <v>126</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H70" s="6"/>
+      <c r="C70" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
       <c r="I70" s="8"/>
     </row>
     <row r="71" spans="1:9">
@@ -2926,31 +3002,29 @@
         <v>130</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>21</v>
+        <v>131</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E71" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="D71" s="5"/>
+      <c r="E71" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F71" s="5"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G71" s="6"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="8"/>
     </row>
     <row r="72" spans="1:9">
-      <c r="A72" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B72" s="8" t="s">
+      <c r="A72" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="B72" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C72" s="5" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -2960,82 +3034,78 @@
       <c r="I72" s="8"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B73" s="5" t="s">
+      <c r="A73" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
+      <c r="B73" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
       <c r="G73" s="8"/>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
+      <c r="G74" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H74" s="6"/>
       <c r="I74" s="8"/>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
-      <c r="G75" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H75" s="6"/>
-      <c r="I75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="76" spans="1:9">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C76" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
-      <c r="I76" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="I76" s="8"/>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="4" t="s">
@@ -3045,7 +3115,7 @@
         <v>140</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>14</v>
@@ -3053,7 +3123,7 @@
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
+      <c r="H77" s="7"/>
       <c r="I77" s="7" t="s">
         <v>14</v>
       </c>
@@ -3063,37 +3133,37 @@
         <v>141</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
+      <c r="E78" s="6"/>
       <c r="F78" s="5"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
+      <c r="G78" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="7"/>
       <c r="I78" s="8"/>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>143</v>
+        <v>24</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="D79" s="5"/>
-      <c r="E79" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="E79" s="5"/>
       <c r="F79" s="5"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G79" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" s="8"/>
       <c r="I79" s="8"/>
     </row>
     <row r="80" spans="1:9">
@@ -3101,38 +3171,36 @@
         <v>144</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>145</v>
+        <v>24</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="D80" s="5"/>
-      <c r="E80" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="E80" s="5"/>
       <c r="F80" s="5"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G80" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="6"/>
       <c r="I80" s="8"/>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D81" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E81" s="5"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="F81" s="5"/>
+      <c r="G81" s="8"/>
       <c r="H81" s="8"/>
       <c r="I81" s="7" t="s">
         <v>14</v>
@@ -3140,34 +3208,34 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>148</v>
-      </c>
       <c r="C82" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E82" s="5"/>
       <c r="F82" s="5"/>
       <c r="G82" s="8"/>
-      <c r="H82" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I82" s="7"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="9" t="s">
-        <v>149</v>
+      <c r="A83" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
@@ -3178,36 +3246,40 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
+      <c r="E84" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F84" s="5"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="7"/>
       <c r="I84" s="8"/>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>151</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
+      <c r="E85" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F85" s="5"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="7"/>
       <c r="I85" s="8"/>
     </row>
     <row r="86" spans="1:9">
@@ -3215,72 +3287,80 @@
         <v>152</v>
       </c>
       <c r="B86" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D86" s="5"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" s="8"/>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>154</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
+      <c r="E87" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F87" s="5"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="I87" s="8"/>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B88" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
+      <c r="B88" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="5"/>
       <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
+      <c r="H88" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="I88" s="8"/>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="9" t="s">
-        <v>156</v>
+      <c r="A89" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D89" s="5"/>
       <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="8"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="H89" s="8"/>
       <c r="I89" s="7" t="s">
         <v>14</v>
@@ -3288,182 +3368,196 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>24</v>
+        <v>159</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
+      <c r="E90" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="8"/>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8"/>
+      <c r="H90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" s="7"/>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
+        <v>160</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>160</v>
+      <c r="A92" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
+      <c r="E92" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F92" s="5"/>
       <c r="G92" s="8"/>
       <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
+      <c r="I92" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>21</v>
+        <v>162</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D93" s="5"/>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="8"/>
       <c r="H93" s="8"/>
-      <c r="I93" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="I93" s="8"/>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
+      <c r="A94" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
+      <c r="I94" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="4" t="s">
-        <v>163</v>
+      <c r="A95" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
-      <c r="G95" s="8"/>
+      <c r="G95" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H95" s="8"/>
       <c r="I95" s="8"/>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D96" s="8"/>
+        <v>69</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="E96" s="8"/>
       <c r="F96" s="8"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
+      <c r="I96" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>167</v>
+      <c r="B97" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D97" s="8"/>
-      <c r="E97" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F97" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
       <c r="G97" s="8"/>
-      <c r="H97" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I97" s="8"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="9" t="s">
+      <c r="A98" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="B98" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="8"/>
       <c r="H98" s="8"/>
       <c r="I98" s="8"/>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B99" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B99" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C99" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
-      <c r="G99" s="8"/>
-      <c r="H99" s="8"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
       <c r="I99" s="8"/>
     </row>
     <row r="100" spans="1:9">
@@ -3471,37 +3565,33 @@
         <v>171</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>92</v>
+        <v>171</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="8"/>
       <c r="F100" s="8"/>
-      <c r="G100" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="G100" s="8"/>
       <c r="H100" s="8"/>
       <c r="I100" s="8"/>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="8" t="s">
         <v>173</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
       <c r="F101" s="5"/>
-      <c r="G101" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H101" s="6"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
       <c r="I101" s="8"/>
     </row>
     <row r="102" spans="1:9">
@@ -3509,29 +3599,31 @@
         <v>174</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D102" s="5"/>
-      <c r="E102" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E102" s="5"/>
       <c r="F102" s="5"/>
-      <c r="G102" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="G102" s="8"/>
       <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
+      <c r="I102" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="4" t="s">
         <v>175</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="D103" s="5"/>
       <c r="E103" s="6" t="s">
@@ -3539,13 +3631,281 @@
       </c>
       <c r="F103" s="5"/>
       <c r="G103" s="6"/>
-      <c r="H103" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="H103" s="7"/>
       <c r="I103" s="8"/>
     </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="8"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D107" s="8"/>
+      <c r="E107" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" s="8"/>
+      <c r="G107" s="8"/>
+      <c r="H107" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" s="8"/>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+      <c r="G108" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H108" s="8"/>
+      <c r="I108" s="8"/>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="8"/>
+      <c r="H109" s="8"/>
+      <c r="I109" s="8"/>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8"/>
+      <c r="G110" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8"/>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H111" s="6"/>
+      <c r="I111" s="8"/>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D112" s="5"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H112" s="8"/>
+      <c r="I112" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D113" s="5"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H113" s="6"/>
+      <c r="I113" s="8"/>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D114" s="5"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" s="6"/>
+      <c r="H114" s="7"/>
+      <c r="I114" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D115" s="5"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H115" s="7"/>
+      <c r="I115" s="8"/>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D116" s="5"/>
+      <c r="E116" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F116" s="5"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I116" s="8"/>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H117" s="6"/>
+      <c r="I117" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I103"/>
+  <autoFilter ref="A2:I117">
+    <sortState ref="A3:I117">
+      <sortCondition ref="A2"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A3:I103">
     <sortCondition ref="A3:A103"/>
   </sortState>
@@ -3557,103 +3917,110 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A69" r:id="rId1" display="PlayCanvas"/>
-    <hyperlink ref="A94" r:id="rId2" display="Turbulenz"/>
-    <hyperlink ref="A26" r:id="rId3" display="D3"/>
-    <hyperlink ref="A63" r:id="rId4" display="OSG.JS"/>
-    <hyperlink ref="A67" r:id="rId5" display="PhiloGL"/>
-    <hyperlink ref="A91" r:id="rId6" display="Three.js"/>
-    <hyperlink ref="A11" r:id="rId7" display="Babylon.js"/>
-    <hyperlink ref="A72" r:id="rId8" display="Processing"/>
-    <hyperlink ref="A32" r:id="rId9" display="Echarts"/>
-    <hyperlink ref="A92" r:id="rId10" display="Timeline"/>
-    <hyperlink ref="A48" r:id="rId11" display="JointJS"/>
-    <hyperlink ref="A40" r:id="rId12" display="Heatmap.js"/>
-    <hyperlink ref="A100" r:id="rId13" display="VTK"/>
-    <hyperlink ref="A65" r:id="rId14" display="ParaView"/>
-    <hyperlink ref="A47" r:id="rId15" display="ITK"/>
-    <hyperlink ref="A98" r:id="rId16" display="Visit"/>
-    <hyperlink ref="A66" r:id="rId17" display="PCL"/>
-    <hyperlink ref="A19" r:id="rId18" display="Cl3ver"/>
-    <hyperlink ref="A43" r:id="rId19" display="HOOPS"/>
-    <hyperlink ref="A38" r:id="rId20" display="GrabCAD"/>
-    <hyperlink ref="A85" r:id="rId21" display="SketchFab"/>
-    <hyperlink ref="A64" r:id="rId22" display="P3D.in"/>
-    <hyperlink ref="A12" r:id="rId23" display="Blend4Web"/>
-    <hyperlink ref="A20" r:id="rId24" display="Clara.io"/>
-    <hyperlink ref="A49" r:id="rId25" display="Lagoa"/>
-    <hyperlink ref="A55" r:id="rId26" display="Meshmixer"/>
-    <hyperlink ref="A93" r:id="rId27" display="Tinkercad"/>
-    <hyperlink ref="A81" r:id="rId28" display="Shapeshifter"/>
-    <hyperlink ref="A21" r:id="rId29" display="ClayTools"/>
-    <hyperlink ref="A46" r:id="rId30" display="IronCAD"/>
-    <hyperlink ref="A73" r:id="rId31" display="PTC Creo"/>
-    <hyperlink ref="A41" r:id="rId32" display="HomeByMe"/>
-    <hyperlink ref="A90" r:id="rId33" display="Solidworks Visualization"/>
-    <hyperlink ref="A7" r:id="rId34" display="3DXcite DELTAGEN"/>
-    <hyperlink ref="A89" r:id="rId35" display="Solidworks"/>
-    <hyperlink ref="A16" r:id="rId36" display="CATIA"/>
-    <hyperlink ref="A29" r:id="rId37" display="DraftSight"/>
-    <hyperlink ref="A60" r:id="rId38" display="NX"/>
-    <hyperlink ref="A99" r:id="rId39" display="VRED Professional"/>
-    <hyperlink ref="A84" r:id="rId40" display="SketchBook Pro"/>
-    <hyperlink ref="A76" r:id="rId41" display="Revit"/>
-    <hyperlink ref="A68" r:id="rId42" display="PIXLR"/>
-    <hyperlink ref="A74" r:id="rId43" display="Recap"/>
-    <hyperlink ref="A57" r:id="rId44" display="Mudbox"/>
-    <hyperlink ref="A53" r:id="rId45" display="Maya"/>
-    <hyperlink ref="A45" r:id="rId46" display="Inventor"/>
-    <hyperlink ref="A42" r:id="rId47" display="Homestyler"/>
-    <hyperlink ref="A37" r:id="rId48" display="Fusion 360"/>
-    <hyperlink ref="A9" r:id="rId49" display="AutoCAD Design Suite"/>
-    <hyperlink ref="A6" r:id="rId50" display="3ds Max Design"/>
-    <hyperlink ref="A8" r:id="rId51" display="Alias Design"/>
-    <hyperlink ref="A36" r:id="rId52" display="Freeform Plus"/>
-    <hyperlink ref="A28" r:id="rId53" display="DesignX"/>
-    <hyperlink ref="A103" r:id="rId54" display="Zbrush"/>
-    <hyperlink ref="A79" r:id="rId55" display="Sculptris"/>
-    <hyperlink ref="A56" r:id="rId56" display="Modo"/>
-    <hyperlink ref="A59" r:id="rId57" display="Nuke Studio"/>
-    <hyperlink ref="A52" r:id="rId58" display="Mari"/>
-    <hyperlink ref="A13" r:id="rId59" display="Blender"/>
-    <hyperlink ref="A70" r:id="rId60" display="PolyWorks"/>
-    <hyperlink ref="A15" r:id="rId61" display="Carrara Pro"/>
-    <hyperlink ref="A27" r:id="rId62" display="DAZ Studio Pro"/>
-    <hyperlink ref="A18" r:id="rId63" display="Cinema 4D Studio"/>
-    <hyperlink ref="A14" r:id="rId64" display="Body Paint"/>
-    <hyperlink ref="A22" r:id="rId65" display="Cobalt"/>
-    <hyperlink ref="A34" r:id="rId66" display="Form-Z Pro"/>
-    <hyperlink ref="A50" r:id="rId67" display="LightWave"/>
-    <hyperlink ref="A17" r:id="rId68" display="ChronoSculpt"/>
-    <hyperlink ref="A77" r:id="rId69" display="Rhino"/>
-    <hyperlink ref="A80" r:id="rId70" display="Shade 3D Pro"/>
-    <hyperlink ref="A82" r:id="rId71" display="Silo"/>
-    <hyperlink ref="A86" r:id="rId72" display="SketchUp"/>
-    <hyperlink ref="A44" r:id="rId73" display="Inspire"/>
-    <hyperlink ref="A33" r:id="rId74" display="Evolve"/>
-    <hyperlink ref="A101" r:id="rId75" display="VXmodel "/>
-    <hyperlink ref="A75" r:id="rId76" display="Remake"/>
-    <hyperlink ref="A54" r:id="rId77" display="MeshLab"/>
-    <hyperlink ref="A58" r:id="rId78" display="Netfabb"/>
-    <hyperlink ref="A4" r:id="rId79" display="3D-matic"/>
-    <hyperlink ref="A5" r:id="rId80" display="3DReshaper"/>
-    <hyperlink ref="A25" r:id="rId81" display="Cura"/>
-    <hyperlink ref="A23" r:id="rId82" display="CraftWare"/>
-    <hyperlink ref="A35" r:id="rId83" display="FreeCAD"/>
-    <hyperlink ref="A83" r:id="rId84" display="Simplify3D"/>
-    <hyperlink ref="A87" r:id="rId85" display="Slic3r"/>
-    <hyperlink ref="A62" r:id="rId86" display="OnShape"/>
-    <hyperlink ref="A97" r:id="rId87" display="Vectary"/>
-    <hyperlink ref="A95" r:id="rId88" display="Unity Pro"/>
-    <hyperlink ref="A96" r:id="rId89" display="Unreal Engine"/>
-    <hyperlink ref="A78" r:id="rId90" display="Scaleform"/>
-    <hyperlink ref="A51" r:id="rId91" display="Lumberyard"/>
-    <hyperlink ref="A61" r:id="rId92" display="OGRE"/>
-    <hyperlink ref="A10" r:id="rId93" display="Away3D"/>
-    <hyperlink ref="A88" r:id="rId94" display="SolidEdge 2D"/>
-    <hyperlink ref="A71" r:id="rId95" display="PowerShape"/>
-    <hyperlink ref="A30" r:id="rId96" display="Dreamcatcher"/>
-    <hyperlink ref="A102" r:id="rId97" display="Within"/>
+    <hyperlink ref="A73" r:id="rId1" display="PlayCanvas"/>
+    <hyperlink ref="A104" r:id="rId2" display="Turbulenz"/>
+    <hyperlink ref="A28" r:id="rId3" display="D3"/>
+    <hyperlink ref="A66" r:id="rId4" display="OSG.JS"/>
+    <hyperlink ref="A70" r:id="rId5" display="PhiloGL"/>
+    <hyperlink ref="A100" r:id="rId6" display="Three.js"/>
+    <hyperlink ref="A13" r:id="rId7" display="Babylon.js"/>
+    <hyperlink ref="A76" r:id="rId8" display="Processing"/>
+    <hyperlink ref="A34" r:id="rId9" display="Echarts"/>
+    <hyperlink ref="A101" r:id="rId10" display="Timeline"/>
+    <hyperlink ref="A51" r:id="rId11" display="JointJS"/>
+    <hyperlink ref="A42" r:id="rId12" display="Heatmap.js"/>
+    <hyperlink ref="A110" r:id="rId13" display="VTK"/>
+    <hyperlink ref="A68" r:id="rId14" display="ParaView"/>
+    <hyperlink ref="A49" r:id="rId15" display="ITK"/>
+    <hyperlink ref="A108" r:id="rId16" display="Visit"/>
+    <hyperlink ref="A69" r:id="rId17" display="PCL"/>
+    <hyperlink ref="A22" r:id="rId18" display="Cl3ver"/>
+    <hyperlink ref="A45" r:id="rId19" display="HOOPS"/>
+    <hyperlink ref="A40" r:id="rId20" display="GrabCAD"/>
+    <hyperlink ref="A93" r:id="rId21" display="SketchFab"/>
+    <hyperlink ref="A67" r:id="rId22" display="P3D.in"/>
+    <hyperlink ref="A14" r:id="rId23" display="Blend4Web"/>
+    <hyperlink ref="A23" r:id="rId24" display="Clara.io"/>
+    <hyperlink ref="A52" r:id="rId25" display="Lagoa"/>
+    <hyperlink ref="A58" r:id="rId26" display="Meshmixer"/>
+    <hyperlink ref="A102" r:id="rId27" display="Tinkercad"/>
+    <hyperlink ref="A89" r:id="rId28" display="Shapeshifter"/>
+    <hyperlink ref="A86" r:id="rId29" display="Sculpt"/>
+    <hyperlink ref="A48" r:id="rId30" display="IronCAD"/>
+    <hyperlink ref="A77" r:id="rId31" display="PTC Creo"/>
+    <hyperlink ref="A43" r:id="rId32" display="HomeByMe"/>
+    <hyperlink ref="A98" r:id="rId33" display="Solidworks Visualization"/>
+    <hyperlink ref="A8" r:id="rId34" display="3DXcite DELTAGEN"/>
+    <hyperlink ref="A97" r:id="rId35" display="Solidworks"/>
+    <hyperlink ref="A18" r:id="rId36" display="CATIA"/>
+    <hyperlink ref="A31" r:id="rId37" display="DraftSight"/>
+    <hyperlink ref="A63" r:id="rId38" display="NX"/>
+    <hyperlink ref="A109" r:id="rId39" display="VRED Professional"/>
+    <hyperlink ref="A92" r:id="rId40" display="SketchBook Pro"/>
+    <hyperlink ref="A81" r:id="rId41" display="Revit"/>
+    <hyperlink ref="A72" r:id="rId42" display="PIXLR"/>
+    <hyperlink ref="A79" r:id="rId43" display="Recap"/>
+    <hyperlink ref="A60" r:id="rId44" display="Mudbox"/>
+    <hyperlink ref="A56" r:id="rId45" display="Maya"/>
+    <hyperlink ref="A47" r:id="rId46" display="Inventor"/>
+    <hyperlink ref="A44" r:id="rId47" display="Homestyler"/>
+    <hyperlink ref="A39" r:id="rId48" display="Fusion 360"/>
+    <hyperlink ref="A11" r:id="rId49" display="AutoCAD Design Suite"/>
+    <hyperlink ref="A7" r:id="rId50" display="3ds Max Design"/>
+    <hyperlink ref="A10" r:id="rId51" display="Alias Design"/>
+    <hyperlink ref="A38" r:id="rId52" display="Freeform"/>
+    <hyperlink ref="A30" r:id="rId53" display="DesignX"/>
+    <hyperlink ref="A116" r:id="rId54" display="Zbrush"/>
+    <hyperlink ref="A87" r:id="rId55" display="Sculptris"/>
+    <hyperlink ref="A59" r:id="rId56" display="Modo"/>
+    <hyperlink ref="A62" r:id="rId57" display="Nuke Studio"/>
+    <hyperlink ref="A55" r:id="rId58" display="Mari"/>
+    <hyperlink ref="A15" r:id="rId59" display="Blender"/>
+    <hyperlink ref="A74" r:id="rId60" display="PolyWorks"/>
+    <hyperlink ref="A17" r:id="rId61" display="Carrara Pro"/>
+    <hyperlink ref="A29" r:id="rId62" display="DAZ Studio Pro"/>
+    <hyperlink ref="A21" r:id="rId63" display="Cinema 4D Studio"/>
+    <hyperlink ref="A16" r:id="rId64" display="Body Paint"/>
+    <hyperlink ref="A24" r:id="rId65" display="Cobalt"/>
+    <hyperlink ref="A36" r:id="rId66" display="Form-Z Pro"/>
+    <hyperlink ref="A53" r:id="rId67" display="LightWave"/>
+    <hyperlink ref="A19" r:id="rId68" display="ChronoSculpt"/>
+    <hyperlink ref="A82" r:id="rId69" display="Rhino"/>
+    <hyperlink ref="A88" r:id="rId70" display="Shade 3D Pro"/>
+    <hyperlink ref="A90" r:id="rId71" display="Silo"/>
+    <hyperlink ref="A94" r:id="rId72" display="SketchUp"/>
+    <hyperlink ref="A46" r:id="rId73" display="Inspire"/>
+    <hyperlink ref="A35" r:id="rId74" display="Evolve"/>
+    <hyperlink ref="A111" r:id="rId75" display="VXmodel "/>
+    <hyperlink ref="A80" r:id="rId76" display="Remake"/>
+    <hyperlink ref="A57" r:id="rId77" display="MeshLab"/>
+    <hyperlink ref="A61" r:id="rId78" display="Netfabb"/>
+    <hyperlink ref="A5" r:id="rId79" display="3D-matic"/>
+    <hyperlink ref="A6" r:id="rId80" display="3DReshaper"/>
+    <hyperlink ref="A27" r:id="rId81" display="Cura"/>
+    <hyperlink ref="A25" r:id="rId82" display="CraftWare"/>
+    <hyperlink ref="A37" r:id="rId83" display="FreeCAD"/>
+    <hyperlink ref="A91" r:id="rId84" display="Simplify3D"/>
+    <hyperlink ref="A95" r:id="rId85" display="Slic3r"/>
+    <hyperlink ref="A65" r:id="rId86" display="OnShape"/>
+    <hyperlink ref="A107" r:id="rId87" display="Vectary"/>
+    <hyperlink ref="A105" r:id="rId88" display="Unity Pro"/>
+    <hyperlink ref="A106" r:id="rId89" display="Unreal Engine"/>
+    <hyperlink ref="A83" r:id="rId90" display="Scaleform"/>
+    <hyperlink ref="A54" r:id="rId91" display="Lumberyard"/>
+    <hyperlink ref="A64" r:id="rId92" display="OGRE"/>
+    <hyperlink ref="A12" r:id="rId93" display="Away3D"/>
+    <hyperlink ref="A96" r:id="rId94" display="SolidEdge 2D"/>
+    <hyperlink ref="A75" r:id="rId95" display="PowerShape"/>
+    <hyperlink ref="A32" r:id="rId96" display="Dreamcatcher"/>
+    <hyperlink ref="A112" r:id="rId97" display="Within"/>
+    <hyperlink ref="A71" r:id="rId98" display="Photoscan"/>
+    <hyperlink ref="A84" r:id="rId99" display="Scandy"/>
+    <hyperlink ref="A85" r:id="rId100" display="Scann3D"/>
+    <hyperlink ref="A103" r:id="rId101" display="Trimensional"/>
+    <hyperlink ref="A78" r:id="rId102" display="RealityCapture"/>
+    <hyperlink ref="A117" r:id="rId103" display="Zephyr"/>
+    <hyperlink ref="A99" r:id="rId104" display="Source SDK"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>